<commit_message>
Logic build to create account groups and accounts from Excel sheet
</commit_message>
<xml_diff>
--- a/public/trial.xlsx
+++ b/public/trial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">Account Type</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">opening credit</t>
   </si>
   <si>
-    <t xml:space="preserve">Asset</t>
+    <t xml:space="preserve">Assets</t>
   </si>
   <si>
     <t xml:space="preserve">Current Asset</t>
@@ -83,6 +83,45 @@
   </si>
   <si>
     <t xml:space="preserve">Equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long Term Liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short Term Liabilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short Term Loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts Payables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. A/P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales &amp; Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales – Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating Expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salaries &amp; Wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilities</t>
   </si>
 </sst>
 </file>
@@ -179,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,6 +229,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -273,16 +316,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
@@ -401,6 +444,71 @@
         <v>20</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
create trial table and fill it with the excel data
</commit_message>
<xml_diff>
--- a/public/trial.xlsx
+++ b/public/trial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">Account Type</t>
   </si>
@@ -41,6 +41,38 @@
   </si>
   <si>
     <t xml:space="preserve">opening credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current movement debt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">current movement</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> credit</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">closing debt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closing credit</t>
   </si>
   <si>
     <t xml:space="preserve">Assets</t>
@@ -164,8 +196,9 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -227,15 +260,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -316,10 +349,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -331,8 +364,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -357,156 +394,210 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+      <c r="A2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="C5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="E6" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>10000</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <v>15000</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>30000</v>
       </c>
+      <c r="K7" s="0" t="n">
+        <v>6000</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="3" t="s">
-        <v>14</v>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>500000</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>55000</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>4500</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>9500</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>500</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>8000</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>8500</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>6000</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>2300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logout button, accounts and account groups folders generating from excel file upload
</commit_message>
<xml_diff>
--- a/public/trial.xlsx
+++ b/public/trial.xlsx
@@ -46,27 +46,7 @@
     <t xml:space="preserve">current movement debt</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">current movement</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> credit</t>
-    </r>
+    <t xml:space="preserve">current movement credit</t>
   </si>
   <si>
     <t xml:space="preserve">closing debt</t>
@@ -84,7 +64,7 @@
     <t xml:space="preserve">Stock</t>
   </si>
   <si>
-    <t xml:space="preserve">A/C Receivable</t>
+    <t xml:space="preserve">Account Receivable</t>
   </si>
   <si>
     <t xml:space="preserve">Mr. X</t>
@@ -164,7 +144,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -194,13 +174,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -251,16 +224,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -351,8 +320,8 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -397,7 +366,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -408,30 +377,30 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
+      <c r="A3" s="2"/>
       <c r="B3" s="0" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
+      <c r="A4" s="2"/>
       <c r="C4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
       <c r="C5" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
+      <c r="A6" s="2"/>
       <c r="E6" s="0" t="s">
         <v>15</v>
       </c>
@@ -462,7 +431,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -516,7 +485,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel recursive account group generation embedded
</commit_message>
<xml_diff>
--- a/public/trial.xlsx
+++ b/public/trial.xlsx
@@ -318,10 +318,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,6 +569,10 @@
         <v>2300</v>
       </c>
     </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>